<commit_message>
Quicker messages update. Pastes rather than typing
</commit_message>
<xml_diff>
--- a/recepient_db.xlsx
+++ b/recepient_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSC Guest\Documents\Shrijan\WhatsAppAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD73831C-566E-4469-B4A5-6923524C9D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C53582C-F953-4D4F-99ED-27F9886FC521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37215" yWindow="3495" windowWidth="16125" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>greeting</t>
   </si>
@@ -51,13 +51,139 @@
     <t>group_id</t>
   </si>
   <si>
-    <t>shrijan</t>
-  </si>
-  <si>
-    <t>+60174808794</t>
-  </si>
-  <si>
-    <t>JwXJuPeIj8Q9cMpqflxYnl</t>
+    <t>Kavish</t>
+  </si>
+  <si>
+    <t>kvishrock120809@gmail.com</t>
+  </si>
+  <si>
+    <t>+60125262136</t>
+  </si>
+  <si>
+    <t>GFlriDI5wB4FhyBqCygwPB</t>
+  </si>
+  <si>
+    <t>Kavish &amp; Hehmaa</t>
+  </si>
+  <si>
+    <t>Hehmaa</t>
+  </si>
+  <si>
+    <t>kaushi180370@gmail.com</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>dss.batuncang@gmail.com</t>
+  </si>
+  <si>
+    <t>+60198188727</t>
+  </si>
+  <si>
+    <t>DxsC8kOzmM80ZUKgPGzrIw</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Samuil-Ashton</t>
+  </si>
+  <si>
+    <t>samsatu@gmail.com</t>
+  </si>
+  <si>
+    <t>+60138362370</t>
+  </si>
+  <si>
+    <t>Shan</t>
+  </si>
+  <si>
+    <t>shanredai@gmail.com</t>
+  </si>
+  <si>
+    <t>+919740081143</t>
+  </si>
+  <si>
+    <t>BXVVhuHWqZkJwOaM1jARrG</t>
+  </si>
+  <si>
+    <t>Priyakari</t>
+  </si>
+  <si>
+    <t>ramadevu.priyakari@gmail.com</t>
+  </si>
+  <si>
+    <t>+919441788160</t>
+  </si>
+  <si>
+    <t>JjqgTyDwbxfFUQsHfAuoty</t>
+  </si>
+  <si>
+    <t>Sudiksha</t>
+  </si>
+  <si>
+    <t>chsudiksha3@gmail.com</t>
+  </si>
+  <si>
+    <t>+919880874620</t>
+  </si>
+  <si>
+    <t>HEnZ5UBNjh60r2fsAU3Ci4</t>
+  </si>
+  <si>
+    <t>Satwik</t>
+  </si>
+  <si>
+    <t>apparasu1966@gmail.com</t>
+  </si>
+  <si>
+    <t>+919866124793</t>
+  </si>
+  <si>
+    <t>B5B4TDTMwnx4NZ7xTd3WBE</t>
+  </si>
+  <si>
+    <t>Kushal</t>
+  </si>
+  <si>
+    <t>kingkushalraj22@gmail.com</t>
+  </si>
+  <si>
+    <t>+601169239511</t>
+  </si>
+  <si>
+    <t>IUPuVg78fcA6Sh7CQWNxmf</t>
+  </si>
+  <si>
+    <t>Radha</t>
+  </si>
+  <si>
+    <t>radhachaganti112@gmail.com</t>
+  </si>
+  <si>
+    <t>+919491392460</t>
+  </si>
+  <si>
+    <t>FOkOvmWcghgDBrm2VUhlOi</t>
+  </si>
+  <si>
+    <t>Guventhra</t>
+  </si>
+  <si>
+    <t>+60102701163</t>
+  </si>
+  <si>
+    <t>Vamsi Krishna</t>
+  </si>
+  <si>
+    <t>+918500970197</t>
+  </si>
+  <si>
+    <t>DVUkMcwQH0k1dlYfAKHvzQ</t>
+  </si>
+  <si>
+    <t>Ms Shan</t>
   </si>
 </sst>
 </file>
@@ -421,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,25 +586,234 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{824089D8-C1E4-4DFF-AC63-6CF152C5566E}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{01FAEA05-CFB6-45AF-9558-80DBE6EED8F6}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{F588B96C-A9BC-49B5-91B0-FF3FC00CF736}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{D99A27BC-FE5E-494A-ABAC-6B5D388E813C}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{02B81AAF-DC65-411E-9EEA-CAFC150F4549}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{75DDE394-D62C-468B-BF73-F14E261FCE58}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>